<commit_message>
Add In-Game QA sheet
</commit_message>
<xml_diff>
--- a/Documentation/siPhone - QA Documentation.xlsx
+++ b/Documentation/siPhone - QA Documentation.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\2223-educational-traveling-sifon\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865261B8-2787-4D41-9857-C9480AD210F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C736E74E-7924-43BE-A8F3-D00E081D4FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D648CD92-32B6-4C0F-8E07-AD7407C26C4A}"/>
+    <workbookView xWindow="9630" yWindow="810" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{D648CD92-32B6-4C0F-8E07-AD7407C26C4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Menu" sheetId="1" r:id="rId1"/>
     <sheet name="Character Carousel" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="In-Game" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="58">
   <si>
     <t>Details</t>
   </si>
@@ -118,19 +118,100 @@
     <t>siPhone - QA Documentation [Main Menu]</t>
   </si>
   <si>
-    <t>Upon clicking the selecting a character and pressing the play button the game map should render.</t>
-  </si>
-  <si>
     <t>siPhone - QA Documentation [Character Carousel]</t>
   </si>
   <si>
     <t>Game map renders.</t>
   </si>
   <si>
-    <t>Checking if selecting a character and beginning to play renders the map</t>
-  </si>
-  <si>
     <t>TEST CASE 4</t>
+  </si>
+  <si>
+    <t>siPhone - QA Documentation [In-Game]</t>
+  </si>
+  <si>
+    <t>TEST CASE 5</t>
+  </si>
+  <si>
+    <t>Carousel</t>
+  </si>
+  <si>
+    <t>Upon selecting a character and pressing the play button the game is successfully started.</t>
+  </si>
+  <si>
+    <t>Game loads successfully.</t>
+  </si>
+  <si>
+    <t>Checking if selecting a character and beginning to play loads the game properly.</t>
+  </si>
+  <si>
+    <t>Map Renderer</t>
+  </si>
+  <si>
+    <t>A map which visualises the loaded GeoJSON from the mappack.</t>
+  </si>
+  <si>
+    <t>Checking if the map visualises properly.</t>
+  </si>
+  <si>
+    <t>TEST CASE 6</t>
+  </si>
+  <si>
+    <t>Status View</t>
+  </si>
+  <si>
+    <t>Shows all resources and winning probability along with the won/lost ratio in the left bottom corner.</t>
+  </si>
+  <si>
+    <t>Properly load in the bottom left corner.</t>
+  </si>
+  <si>
+    <t>Checking if the status view loads properly and displays correct data.</t>
+  </si>
+  <si>
+    <t>TEST CASE 7</t>
+  </si>
+  <si>
+    <t>TEST CASE 8</t>
+  </si>
+  <si>
+    <t>Action Button(Organisation)</t>
+  </si>
+  <si>
+    <t>Puts you in organisation mode so you can click on a country on the map to make an organisation on it.</t>
+  </si>
+  <si>
+    <t>Successfully creates an organisation.</t>
+  </si>
+  <si>
+    <t>Check if Organisation Action Button successfully creates an oraganisation.</t>
+  </si>
+  <si>
+    <t>Action Button(Revolution)</t>
+  </si>
+  <si>
+    <t>Makes a national revolution, if the calculations are over a certaing winning threshold the revolution is successful.</t>
+  </si>
+  <si>
+    <t>Successfully makes a national revolution.</t>
+  </si>
+  <si>
+    <t>Checking if starting a national revolution is successful and checking if going over a certain threshold results in a win.</t>
+  </si>
+  <si>
+    <t>Action Button(Resources)</t>
+  </si>
+  <si>
+    <t>Leads to another menu which lets you buy different resources which make the chance of winning higher.</t>
+  </si>
+  <si>
+    <t>TEST CASE 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opens menu successfully. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checking if the resources menu opens successfully. </t>
   </si>
 </sst>
 </file>
@@ -387,172 +468,172 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -891,91 +972,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="54"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="2" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="55"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="57"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="16"/>
     </row>
     <row r="3" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="55"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="57"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="16"/>
     </row>
     <row r="4" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D4" s="58"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="60"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="19"/>
     </row>
     <row r="6" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="19"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="22"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C7" s="15"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="22"/>
+      <c r="C7" s="37"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="25"/>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C8" s="15"/>
+      <c r="C8" s="37"/>
       <c r="E8" s="3"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -988,75 +1069,75 @@
       <c r="N8" s="4"/>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C9" s="15"/>
-      <c r="E9" s="23" t="s">
+      <c r="C9" s="37"/>
+      <c r="E9" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="27" t="s">
+      <c r="F9" s="27"/>
+      <c r="G9" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="23" t="s">
+      <c r="H9" s="31"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="24"/>
-      <c r="L9" s="27" t="s">
+      <c r="K9" s="27"/>
+      <c r="L9" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M9" s="28"/>
-      <c r="N9" s="29"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="32"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C10" s="15"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="32"/>
+      <c r="C10" s="37"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="35"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C11" s="15"/>
-      <c r="E11" s="23" t="s">
+      <c r="C11" s="37"/>
+      <c r="E11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="27" t="s">
+      <c r="F11" s="27"/>
+      <c r="G11" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="28"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="23" t="s">
+      <c r="H11" s="31"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="24"/>
-      <c r="L11" s="33" t="s">
+      <c r="K11" s="27"/>
+      <c r="L11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="34"/>
-      <c r="N11" s="35"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="7"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C12" s="15"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="38"/>
+      <c r="C12" s="37"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="10"/>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C13" s="15"/>
+      <c r="C13" s="37"/>
       <c r="E13" s="3"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1069,118 +1150,118 @@
       <c r="N13" s="4"/>
     </row>
     <row r="14" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="15"/>
+      <c r="C14" s="37"/>
       <c r="E14" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="41"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="51"/>
       <c r="H14" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="41"/>
+      <c r="I14" s="51"/>
       <c r="J14" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="41"/>
+      <c r="K14" s="51"/>
       <c r="L14" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="42"/>
-      <c r="N14" s="43"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="41"/>
     </row>
     <row r="15" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="15"/>
-      <c r="E15" s="5" t="s">
+      <c r="C15" s="37"/>
+      <c r="E15" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="44"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="5" t="s">
+      <c r="F15" s="57"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="45"/>
-      <c r="J15" s="5" t="s">
+      <c r="I15" s="52"/>
+      <c r="J15" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="6"/>
-      <c r="L15" s="5" t="s">
+      <c r="K15" s="44"/>
+      <c r="L15" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="11"/>
-      <c r="N15" s="6"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="44"/>
     </row>
     <row r="16" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="15"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="8"/>
+      <c r="C16" s="37"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="46"/>
+      <c r="N16" s="47"/>
     </row>
     <row r="17" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="15"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="8"/>
+      <c r="C17" s="37"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="47"/>
     </row>
     <row r="18" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="16"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="10"/>
+      <c r="C18" s="38"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="50"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="19"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="22"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C24" s="15"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="22"/>
+      <c r="C24" s="37"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="25"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C25" s="15"/>
+      <c r="C25" s="37"/>
       <c r="E25" s="3"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1193,75 +1274,75 @@
       <c r="N25" s="4"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C26" s="15"/>
-      <c r="E26" s="23" t="s">
+      <c r="C26" s="37"/>
+      <c r="E26" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F26" s="24"/>
-      <c r="G26" s="27" t="s">
+      <c r="F26" s="27"/>
+      <c r="G26" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="H26" s="28"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="23" t="s">
+      <c r="H26" s="31"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="K26" s="24"/>
-      <c r="L26" s="27" t="s">
+      <c r="K26" s="27"/>
+      <c r="L26" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M26" s="28"/>
-      <c r="N26" s="29"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="32"/>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C27" s="15"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="32"/>
+      <c r="C27" s="37"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="35"/>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C28" s="15"/>
-      <c r="E28" s="23" t="s">
+      <c r="C28" s="37"/>
+      <c r="E28" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="24"/>
-      <c r="G28" s="27" t="s">
+      <c r="F28" s="27"/>
+      <c r="G28" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="H28" s="28"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="23" t="s">
+      <c r="H28" s="31"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="K28" s="24"/>
-      <c r="L28" s="33" t="s">
+      <c r="K28" s="27"/>
+      <c r="L28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="M28" s="34"/>
-      <c r="N28" s="35"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="7"/>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C29" s="15"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="37"/>
-      <c r="N29" s="38"/>
+      <c r="C29" s="37"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="10"/>
     </row>
     <row r="30" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C30" s="15"/>
+      <c r="C30" s="37"/>
       <c r="E30" s="3"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -1274,118 +1355,118 @@
       <c r="N30" s="4"/>
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C31" s="15"/>
+      <c r="C31" s="37"/>
       <c r="E31" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="40"/>
-      <c r="G31" s="41"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="51"/>
       <c r="H31" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="I31" s="41"/>
+      <c r="I31" s="51"/>
       <c r="J31" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="K31" s="41"/>
+      <c r="K31" s="51"/>
       <c r="L31" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="M31" s="42"/>
-      <c r="N31" s="43"/>
+      <c r="M31" s="40"/>
+      <c r="N31" s="41"/>
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C32" s="15"/>
-      <c r="E32" s="5" t="s">
+      <c r="C32" s="37"/>
+      <c r="E32" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="F32" s="44"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="5" t="s">
+      <c r="F32" s="57"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="I32" s="45"/>
-      <c r="J32" s="5" t="s">
+      <c r="I32" s="52"/>
+      <c r="J32" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="K32" s="6"/>
-      <c r="L32" s="5" t="s">
+      <c r="K32" s="44"/>
+      <c r="L32" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="M32" s="11"/>
-      <c r="N32" s="6"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="44"/>
     </row>
     <row r="33" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C33" s="15"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="46"/>
-      <c r="I33" s="48"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="8"/>
+      <c r="C33" s="37"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="54"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="45"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="47"/>
     </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C34" s="15"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="8"/>
+      <c r="C34" s="37"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="54"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="45"/>
+      <c r="M34" s="46"/>
+      <c r="N34" s="47"/>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C35" s="16"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="51"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="10"/>
+      <c r="C35" s="38"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="50"/>
+      <c r="L35" s="48"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="50"/>
     </row>
     <row r="40" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E40" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="19"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="22"/>
     </row>
     <row r="41" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C41" s="15"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
-      <c r="L41" s="21"/>
-      <c r="M41" s="21"/>
-      <c r="N41" s="22"/>
+      <c r="C41" s="37"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="24"/>
+      <c r="N41" s="25"/>
     </row>
     <row r="42" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C42" s="15"/>
+      <c r="C42" s="37"/>
       <c r="E42" s="3"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -1398,75 +1479,75 @@
       <c r="N42" s="4"/>
     </row>
     <row r="43" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C43" s="15"/>
-      <c r="E43" s="23" t="s">
+      <c r="C43" s="37"/>
+      <c r="E43" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F43" s="24"/>
-      <c r="G43" s="27" t="s">
+      <c r="F43" s="27"/>
+      <c r="G43" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="H43" s="28"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="23" t="s">
+      <c r="H43" s="31"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="K43" s="24"/>
-      <c r="L43" s="27" t="s">
+      <c r="K43" s="27"/>
+      <c r="L43" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M43" s="28"/>
-      <c r="N43" s="29"/>
+      <c r="M43" s="31"/>
+      <c r="N43" s="32"/>
     </row>
     <row r="44" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C44" s="15"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="30"/>
-      <c r="H44" s="31"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="26"/>
-      <c r="L44" s="30"/>
-      <c r="M44" s="31"/>
-      <c r="N44" s="32"/>
+      <c r="C44" s="37"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="33"/>
+      <c r="M44" s="34"/>
+      <c r="N44" s="35"/>
     </row>
     <row r="45" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C45" s="15"/>
-      <c r="E45" s="23" t="s">
+      <c r="C45" s="37"/>
+      <c r="E45" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F45" s="24"/>
-      <c r="G45" s="27" t="s">
+      <c r="F45" s="27"/>
+      <c r="G45" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="H45" s="28"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="23" t="s">
+      <c r="H45" s="31"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="K45" s="24"/>
-      <c r="L45" s="33" t="s">
+      <c r="K45" s="27"/>
+      <c r="L45" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="M45" s="34"/>
-      <c r="N45" s="35"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="7"/>
     </row>
     <row r="46" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C46" s="15"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="30"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="32"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="26"/>
-      <c r="L46" s="36"/>
-      <c r="M46" s="37"/>
-      <c r="N46" s="38"/>
+      <c r="C46" s="37"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="34"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="28"/>
+      <c r="K46" s="29"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="10"/>
     </row>
     <row r="47" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C47" s="15"/>
+      <c r="C47" s="37"/>
       <c r="E47" s="3"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -1479,95 +1560,120 @@
       <c r="N47" s="4"/>
     </row>
     <row r="48" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C48" s="15"/>
+      <c r="C48" s="37"/>
       <c r="E48" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F48" s="40"/>
-      <c r="G48" s="41"/>
+      <c r="F48" s="60"/>
+      <c r="G48" s="51"/>
       <c r="H48" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="I48" s="41"/>
+      <c r="I48" s="51"/>
       <c r="J48" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="K48" s="41"/>
+      <c r="K48" s="51"/>
       <c r="L48" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="M48" s="42"/>
-      <c r="N48" s="43"/>
+      <c r="M48" s="40"/>
+      <c r="N48" s="41"/>
     </row>
     <row r="49" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C49" s="15"/>
-      <c r="E49" s="5" t="s">
+      <c r="C49" s="37"/>
+      <c r="E49" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F49" s="44"/>
-      <c r="G49" s="45"/>
-      <c r="H49" s="5" t="s">
+      <c r="F49" s="57"/>
+      <c r="G49" s="52"/>
+      <c r="H49" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="I49" s="45"/>
-      <c r="J49" s="5" t="s">
+      <c r="I49" s="52"/>
+      <c r="J49" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="K49" s="6"/>
-      <c r="L49" s="5" t="s">
+      <c r="K49" s="44"/>
+      <c r="L49" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="M49" s="11"/>
-      <c r="N49" s="6"/>
+      <c r="M49" s="43"/>
+      <c r="N49" s="44"/>
     </row>
     <row r="50" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C50" s="15"/>
-      <c r="E50" s="46"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="48"/>
-      <c r="H50" s="46"/>
-      <c r="I50" s="48"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="7"/>
-      <c r="M50" s="12"/>
-      <c r="N50" s="8"/>
+      <c r="C50" s="37"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="58"/>
+      <c r="G50" s="54"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="54"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="47"/>
+      <c r="L50" s="45"/>
+      <c r="M50" s="46"/>
+      <c r="N50" s="47"/>
     </row>
     <row r="51" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C51" s="15"/>
-      <c r="E51" s="46"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="48"/>
-      <c r="H51" s="46"/>
-      <c r="I51" s="48"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="12"/>
-      <c r="N51" s="8"/>
+      <c r="C51" s="37"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="58"/>
+      <c r="G51" s="54"/>
+      <c r="H51" s="53"/>
+      <c r="I51" s="54"/>
+      <c r="J51" s="45"/>
+      <c r="K51" s="47"/>
+      <c r="L51" s="45"/>
+      <c r="M51" s="46"/>
+      <c r="N51" s="47"/>
     </row>
     <row r="52" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C52" s="16"/>
-      <c r="E52" s="49"/>
-      <c r="F52" s="50"/>
-      <c r="G52" s="51"/>
-      <c r="H52" s="49"/>
-      <c r="I52" s="51"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="10"/>
-      <c r="L52" s="9"/>
-      <c r="M52" s="13"/>
-      <c r="N52" s="10"/>
+      <c r="C52" s="38"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="59"/>
+      <c r="G52" s="56"/>
+      <c r="H52" s="55"/>
+      <c r="I52" s="56"/>
+      <c r="J52" s="48"/>
+      <c r="K52" s="50"/>
+      <c r="L52" s="48"/>
+      <c r="M52" s="49"/>
+      <c r="N52" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="L11:N12"/>
-    <mergeCell ref="D1:N4"/>
-    <mergeCell ref="E6:N7"/>
-    <mergeCell ref="E9:F10"/>
-    <mergeCell ref="G9:I10"/>
-    <mergeCell ref="J9:K10"/>
-    <mergeCell ref="L9:N10"/>
+    <mergeCell ref="J49:K52"/>
+    <mergeCell ref="L49:N52"/>
+    <mergeCell ref="C40:C52"/>
+    <mergeCell ref="E40:N41"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="G43:I44"/>
+    <mergeCell ref="J43:K44"/>
+    <mergeCell ref="L43:N44"/>
+    <mergeCell ref="E45:F46"/>
+    <mergeCell ref="G45:I46"/>
+    <mergeCell ref="J45:K46"/>
+    <mergeCell ref="L45:N46"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="L48:N48"/>
+    <mergeCell ref="E49:G52"/>
+    <mergeCell ref="H49:I52"/>
+    <mergeCell ref="C23:C35"/>
+    <mergeCell ref="E23:N24"/>
+    <mergeCell ref="E28:F29"/>
+    <mergeCell ref="G28:I29"/>
+    <mergeCell ref="J28:K29"/>
+    <mergeCell ref="L28:N29"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="E32:G35"/>
+    <mergeCell ref="H32:I35"/>
+    <mergeCell ref="J32:K35"/>
+    <mergeCell ref="L32:N35"/>
     <mergeCell ref="E26:F27"/>
     <mergeCell ref="G26:I27"/>
     <mergeCell ref="J26:K27"/>
@@ -1584,38 +1690,13 @@
     <mergeCell ref="E11:F12"/>
     <mergeCell ref="G11:I12"/>
     <mergeCell ref="J11:K12"/>
-    <mergeCell ref="E49:G52"/>
-    <mergeCell ref="H49:I52"/>
-    <mergeCell ref="C23:C35"/>
-    <mergeCell ref="E23:N24"/>
-    <mergeCell ref="E28:F29"/>
-    <mergeCell ref="G28:I29"/>
-    <mergeCell ref="J28:K29"/>
-    <mergeCell ref="L28:N29"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="E32:G35"/>
-    <mergeCell ref="H32:I35"/>
-    <mergeCell ref="J32:K35"/>
-    <mergeCell ref="L32:N35"/>
-    <mergeCell ref="J49:K52"/>
-    <mergeCell ref="L49:N52"/>
-    <mergeCell ref="C40:C52"/>
-    <mergeCell ref="E40:N41"/>
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="G43:I44"/>
-    <mergeCell ref="J43:K44"/>
-    <mergeCell ref="L43:N44"/>
-    <mergeCell ref="E45:F46"/>
-    <mergeCell ref="G45:I46"/>
-    <mergeCell ref="J45:K46"/>
-    <mergeCell ref="L45:N46"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="L48:N48"/>
+    <mergeCell ref="L11:N12"/>
+    <mergeCell ref="D1:N4"/>
+    <mergeCell ref="E6:N7"/>
+    <mergeCell ref="E9:F10"/>
+    <mergeCell ref="G9:I10"/>
+    <mergeCell ref="J9:K10"/>
+    <mergeCell ref="L9:N10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1626,14 +1707,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F036149-7B35-4A10-BE2D-DA1CD8A96F26}">
   <dimension ref="C1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="3.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="3.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
@@ -1646,91 +1727,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D1" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="54"/>
+      <c r="D1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="2" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="55"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="57"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="16"/>
     </row>
     <row r="3" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="55"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="57"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="16"/>
     </row>
     <row r="4" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D4" s="58"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="60"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="19"/>
     </row>
     <row r="6" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="19"/>
+      <c r="E6" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="22"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C7" s="15"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="22"/>
+      <c r="C7" s="37"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="25"/>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C8" s="15"/>
+      <c r="C8" s="37"/>
       <c r="E8" s="3"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1743,75 +1824,75 @@
       <c r="N8" s="4"/>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C9" s="15"/>
-      <c r="E9" s="23" t="s">
+      <c r="C9" s="37"/>
+      <c r="E9" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="23" t="s">
+      <c r="F9" s="27"/>
+      <c r="G9" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="31"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="24"/>
-      <c r="L9" s="27" t="s">
+      <c r="K9" s="27"/>
+      <c r="L9" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M9" s="28"/>
-      <c r="N9" s="29"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="32"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C10" s="15"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="32"/>
+      <c r="C10" s="37"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="35"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C11" s="15"/>
-      <c r="E11" s="23" t="s">
+      <c r="C11" s="37"/>
+      <c r="E11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="27" t="s">
+      <c r="F11" s="27"/>
+      <c r="G11" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="28"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="23" t="s">
+      <c r="H11" s="31"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="24"/>
-      <c r="L11" s="33" t="s">
+      <c r="K11" s="27"/>
+      <c r="L11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="34"/>
-      <c r="N11" s="35"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="7"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C12" s="15"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="38"/>
+      <c r="C12" s="37"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="10"/>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C13" s="15"/>
+      <c r="C13" s="37"/>
       <c r="E13" s="3"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1824,85 +1905,85 @@
       <c r="N13" s="4"/>
     </row>
     <row r="14" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="15"/>
+      <c r="C14" s="37"/>
       <c r="E14" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="41"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="51"/>
       <c r="H14" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="41"/>
+      <c r="I14" s="51"/>
       <c r="J14" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="41"/>
+      <c r="K14" s="51"/>
       <c r="L14" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="42"/>
-      <c r="N14" s="43"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="41"/>
     </row>
     <row r="15" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="15"/>
-      <c r="E15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="44"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="45"/>
-      <c r="J15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K15" s="6"/>
-      <c r="L15" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M15" s="11"/>
-      <c r="N15" s="6"/>
+      <c r="C15" s="37"/>
+      <c r="E15" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="57"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="52"/>
+      <c r="J15" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15" s="44"/>
+      <c r="L15" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="M15" s="43"/>
+      <c r="N15" s="44"/>
     </row>
     <row r="16" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="15"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="8"/>
+      <c r="C16" s="37"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="46"/>
+      <c r="N16" s="47"/>
     </row>
     <row r="17" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="15"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="8"/>
+      <c r="C17" s="37"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="47"/>
     </row>
     <row r="18" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="16"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="10"/>
+      <c r="C18" s="38"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="50"/>
     </row>
     <row r="23" spans="3:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C23"/>
@@ -2326,6 +2407,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D1:N4"/>
+    <mergeCell ref="L11:N12"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:N14"/>
     <mergeCell ref="C6:C18"/>
     <mergeCell ref="E6:N7"/>
     <mergeCell ref="E9:F10"/>
@@ -2339,12 +2426,6 @@
     <mergeCell ref="H15:I18"/>
     <mergeCell ref="J15:K18"/>
     <mergeCell ref="L15:N18"/>
-    <mergeCell ref="D1:N4"/>
-    <mergeCell ref="L11:N12"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:N14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2352,13 +2433,1258 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C05D9BDB-2A0A-4750-82D7-54787D53F606}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE8B6368-A87C-4400-8492-EA4B9352E125}">
+  <dimension ref="B1:N86"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.140625" style="1" customWidth="1"/>
+    <col min="9" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="9.140625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="13"/>
+    </row>
+    <row r="2" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="16"/>
+    </row>
+    <row r="3" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="16"/>
+    </row>
+    <row r="4" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="19"/>
+    </row>
+    <row r="6" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="22"/>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C7" s="37"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="25"/>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C8" s="37"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C9" s="37"/>
+      <c r="E9" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="27"/>
+      <c r="G9" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="31"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="27"/>
+      <c r="L9" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="M9" s="31"/>
+      <c r="N9" s="32"/>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C10" s="37"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="35"/>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C11" s="37"/>
+      <c r="E11" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="27"/>
+      <c r="G11" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="31"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="27"/>
+      <c r="L11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C12" s="37"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="10"/>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C13" s="37"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="37"/>
+      <c r="E14" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="60"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="51"/>
+      <c r="J14" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="51"/>
+      <c r="L14" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="40"/>
+      <c r="N14" s="41"/>
+    </row>
+    <row r="15" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="37"/>
+      <c r="E15" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="57"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="52"/>
+      <c r="J15" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="44"/>
+      <c r="L15" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="M15" s="43"/>
+      <c r="N15" s="44"/>
+    </row>
+    <row r="16" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="37"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="46"/>
+      <c r="N16" s="47"/>
+    </row>
+    <row r="17" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="37"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="47"/>
+    </row>
+    <row r="18" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="38"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="50"/>
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C23" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="22"/>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C24" s="37"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="25"/>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C25" s="37"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="4"/>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C26" s="37"/>
+      <c r="E26" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="27"/>
+      <c r="G26" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" s="31"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" s="27"/>
+      <c r="L26" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="M26" s="31"/>
+      <c r="N26" s="32"/>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C27" s="37"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="35"/>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C28" s="37"/>
+      <c r="E28" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="27"/>
+      <c r="G28" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" s="31"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="K28" s="27"/>
+      <c r="L28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M28" s="6"/>
+      <c r="N28" s="7"/>
+    </row>
+    <row r="29" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C29" s="37"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="10"/>
+    </row>
+    <row r="30" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C30" s="37"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="4"/>
+    </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C31" s="37"/>
+      <c r="E31" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="60"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" s="51"/>
+      <c r="J31" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="K31" s="51"/>
+      <c r="L31" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="M31" s="40"/>
+      <c r="N31" s="41"/>
+    </row>
+    <row r="32" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C32" s="37"/>
+      <c r="E32" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="57"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="I32" s="52"/>
+      <c r="J32" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="K32" s="44"/>
+      <c r="L32" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="M32" s="43"/>
+      <c r="N32" s="44"/>
+    </row>
+    <row r="33" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C33" s="37"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="54"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="45"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="47"/>
+    </row>
+    <row r="34" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C34" s="37"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="54"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="45"/>
+      <c r="M34" s="46"/>
+      <c r="N34" s="47"/>
+    </row>
+    <row r="35" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C35" s="38"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="50"/>
+      <c r="L35" s="48"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="50"/>
+    </row>
+    <row r="36" spans="3:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+    </row>
+    <row r="37" spans="3:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+    </row>
+    <row r="38" spans="3:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+    </row>
+    <row r="39" spans="3:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+    </row>
+    <row r="40" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C40" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="22"/>
+    </row>
+    <row r="41" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C41" s="37"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="24"/>
+      <c r="N41" s="25"/>
+    </row>
+    <row r="42" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C42" s="37"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="4"/>
+    </row>
+    <row r="43" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C43" s="37"/>
+      <c r="E43" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" s="27"/>
+      <c r="G43" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="H43" s="31"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K43" s="27"/>
+      <c r="L43" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="M43" s="31"/>
+      <c r="N43" s="32"/>
+    </row>
+    <row r="44" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C44" s="37"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="33"/>
+      <c r="M44" s="34"/>
+      <c r="N44" s="35"/>
+    </row>
+    <row r="45" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C45" s="37"/>
+      <c r="E45" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="27"/>
+      <c r="G45" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H45" s="31"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="K45" s="27"/>
+      <c r="L45" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M45" s="6"/>
+      <c r="N45" s="7"/>
+    </row>
+    <row r="46" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C46" s="37"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="34"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="28"/>
+      <c r="K46" s="29"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="10"/>
+    </row>
+    <row r="47" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C47" s="37"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="4"/>
+    </row>
+    <row r="48" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C48" s="37"/>
+      <c r="E48" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="60"/>
+      <c r="G48" s="51"/>
+      <c r="H48" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="I48" s="51"/>
+      <c r="J48" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="K48" s="51"/>
+      <c r="L48" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="M48" s="40"/>
+      <c r="N48" s="41"/>
+    </row>
+    <row r="49" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C49" s="37"/>
+      <c r="E49" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="F49" s="57"/>
+      <c r="G49" s="52"/>
+      <c r="H49" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="I49" s="52"/>
+      <c r="J49" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="K49" s="44"/>
+      <c r="L49" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="M49" s="43"/>
+      <c r="N49" s="44"/>
+    </row>
+    <row r="50" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C50" s="37"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="58"/>
+      <c r="G50" s="54"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="54"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="47"/>
+      <c r="L50" s="45"/>
+      <c r="M50" s="46"/>
+      <c r="N50" s="47"/>
+    </row>
+    <row r="51" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C51" s="37"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="58"/>
+      <c r="G51" s="54"/>
+      <c r="H51" s="53"/>
+      <c r="I51" s="54"/>
+      <c r="J51" s="45"/>
+      <c r="K51" s="47"/>
+      <c r="L51" s="45"/>
+      <c r="M51" s="46"/>
+      <c r="N51" s="47"/>
+    </row>
+    <row r="52" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C52" s="38"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="59"/>
+      <c r="G52" s="56"/>
+      <c r="H52" s="55"/>
+      <c r="I52" s="56"/>
+      <c r="J52" s="48"/>
+      <c r="K52" s="50"/>
+      <c r="L52" s="48"/>
+      <c r="M52" s="49"/>
+      <c r="N52" s="50"/>
+    </row>
+    <row r="57" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C57" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="21"/>
+      <c r="J57" s="21"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="21"/>
+      <c r="M57" s="21"/>
+      <c r="N57" s="22"/>
+    </row>
+    <row r="58" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C58" s="37"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="24"/>
+      <c r="J58" s="24"/>
+      <c r="K58" s="24"/>
+      <c r="L58" s="24"/>
+      <c r="M58" s="24"/>
+      <c r="N58" s="25"/>
+    </row>
+    <row r="59" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C59" s="37"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="4"/>
+    </row>
+    <row r="60" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C60" s="37"/>
+      <c r="E60" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F60" s="27"/>
+      <c r="G60" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="H60" s="31"/>
+      <c r="I60" s="32"/>
+      <c r="J60" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K60" s="27"/>
+      <c r="L60" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="M60" s="31"/>
+      <c r="N60" s="32"/>
+    </row>
+    <row r="61" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C61" s="37"/>
+      <c r="E61" s="28"/>
+      <c r="F61" s="29"/>
+      <c r="G61" s="33"/>
+      <c r="H61" s="34"/>
+      <c r="I61" s="35"/>
+      <c r="J61" s="28"/>
+      <c r="K61" s="29"/>
+      <c r="L61" s="33"/>
+      <c r="M61" s="34"/>
+      <c r="N61" s="35"/>
+    </row>
+    <row r="62" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C62" s="37"/>
+      <c r="E62" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" s="27"/>
+      <c r="G62" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H62" s="31"/>
+      <c r="I62" s="32"/>
+      <c r="J62" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="K62" s="27"/>
+      <c r="L62" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M62" s="6"/>
+      <c r="N62" s="7"/>
+    </row>
+    <row r="63" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C63" s="37"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="29"/>
+      <c r="G63" s="33"/>
+      <c r="H63" s="34"/>
+      <c r="I63" s="35"/>
+      <c r="J63" s="28"/>
+      <c r="K63" s="29"/>
+      <c r="L63" s="8"/>
+      <c r="M63" s="9"/>
+      <c r="N63" s="10"/>
+    </row>
+    <row r="64" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C64" s="37"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+      <c r="N64" s="4"/>
+    </row>
+    <row r="65" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C65" s="37"/>
+      <c r="E65" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="60"/>
+      <c r="G65" s="51"/>
+      <c r="H65" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="I65" s="51"/>
+      <c r="J65" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="K65" s="51"/>
+      <c r="L65" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="M65" s="40"/>
+      <c r="N65" s="41"/>
+    </row>
+    <row r="66" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C66" s="37"/>
+      <c r="E66" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="F66" s="57"/>
+      <c r="G66" s="52"/>
+      <c r="H66" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="I66" s="52"/>
+      <c r="J66" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="K66" s="44"/>
+      <c r="L66" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="M66" s="43"/>
+      <c r="N66" s="44"/>
+    </row>
+    <row r="67" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C67" s="37"/>
+      <c r="E67" s="53"/>
+      <c r="F67" s="58"/>
+      <c r="G67" s="54"/>
+      <c r="H67" s="53"/>
+      <c r="I67" s="54"/>
+      <c r="J67" s="45"/>
+      <c r="K67" s="47"/>
+      <c r="L67" s="45"/>
+      <c r="M67" s="46"/>
+      <c r="N67" s="47"/>
+    </row>
+    <row r="68" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C68" s="37"/>
+      <c r="E68" s="53"/>
+      <c r="F68" s="58"/>
+      <c r="G68" s="54"/>
+      <c r="H68" s="53"/>
+      <c r="I68" s="54"/>
+      <c r="J68" s="45"/>
+      <c r="K68" s="47"/>
+      <c r="L68" s="45"/>
+      <c r="M68" s="46"/>
+      <c r="N68" s="47"/>
+    </row>
+    <row r="69" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C69" s="38"/>
+      <c r="E69" s="55"/>
+      <c r="F69" s="59"/>
+      <c r="G69" s="56"/>
+      <c r="H69" s="55"/>
+      <c r="I69" s="56"/>
+      <c r="J69" s="48"/>
+      <c r="K69" s="50"/>
+      <c r="L69" s="48"/>
+      <c r="M69" s="49"/>
+      <c r="N69" s="50"/>
+    </row>
+    <row r="74" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C74" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F74" s="21"/>
+      <c r="G74" s="21"/>
+      <c r="H74" s="21"/>
+      <c r="I74" s="21"/>
+      <c r="J74" s="21"/>
+      <c r="K74" s="21"/>
+      <c r="L74" s="21"/>
+      <c r="M74" s="21"/>
+      <c r="N74" s="22"/>
+    </row>
+    <row r="75" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C75" s="37"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="24"/>
+      <c r="H75" s="24"/>
+      <c r="I75" s="24"/>
+      <c r="J75" s="24"/>
+      <c r="K75" s="24"/>
+      <c r="L75" s="24"/>
+      <c r="M75" s="24"/>
+      <c r="N75" s="25"/>
+    </row>
+    <row r="76" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C76" s="37"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="2"/>
+      <c r="N76" s="4"/>
+    </row>
+    <row r="77" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C77" s="37"/>
+      <c r="E77" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F77" s="27"/>
+      <c r="G77" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="H77" s="31"/>
+      <c r="I77" s="32"/>
+      <c r="J77" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K77" s="27"/>
+      <c r="L77" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="M77" s="31"/>
+      <c r="N77" s="32"/>
+    </row>
+    <row r="78" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C78" s="37"/>
+      <c r="E78" s="28"/>
+      <c r="F78" s="29"/>
+      <c r="G78" s="33"/>
+      <c r="H78" s="34"/>
+      <c r="I78" s="35"/>
+      <c r="J78" s="28"/>
+      <c r="K78" s="29"/>
+      <c r="L78" s="33"/>
+      <c r="M78" s="34"/>
+      <c r="N78" s="35"/>
+    </row>
+    <row r="79" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C79" s="37"/>
+      <c r="E79" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F79" s="27"/>
+      <c r="G79" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H79" s="31"/>
+      <c r="I79" s="32"/>
+      <c r="J79" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="K79" s="27"/>
+      <c r="L79" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M79" s="6"/>
+      <c r="N79" s="7"/>
+    </row>
+    <row r="80" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C80" s="37"/>
+      <c r="E80" s="28"/>
+      <c r="F80" s="29"/>
+      <c r="G80" s="33"/>
+      <c r="H80" s="34"/>
+      <c r="I80" s="35"/>
+      <c r="J80" s="28"/>
+      <c r="K80" s="29"/>
+      <c r="L80" s="8"/>
+      <c r="M80" s="9"/>
+      <c r="N80" s="10"/>
+    </row>
+    <row r="81" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C81" s="37"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2"/>
+      <c r="K81" s="2"/>
+      <c r="L81" s="2"/>
+      <c r="M81" s="2"/>
+      <c r="N81" s="4"/>
+    </row>
+    <row r="82" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C82" s="37"/>
+      <c r="E82" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="60"/>
+      <c r="G82" s="51"/>
+      <c r="H82" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="I82" s="51"/>
+      <c r="J82" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="K82" s="51"/>
+      <c r="L82" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="M82" s="40"/>
+      <c r="N82" s="41"/>
+    </row>
+    <row r="83" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C83" s="37"/>
+      <c r="E83" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="F83" s="57"/>
+      <c r="G83" s="52"/>
+      <c r="H83" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="I83" s="52"/>
+      <c r="J83" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="K83" s="44"/>
+      <c r="L83" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="M83" s="43"/>
+      <c r="N83" s="44"/>
+    </row>
+    <row r="84" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C84" s="37"/>
+      <c r="E84" s="53"/>
+      <c r="F84" s="58"/>
+      <c r="G84" s="54"/>
+      <c r="H84" s="53"/>
+      <c r="I84" s="54"/>
+      <c r="J84" s="45"/>
+      <c r="K84" s="47"/>
+      <c r="L84" s="45"/>
+      <c r="M84" s="46"/>
+      <c r="N84" s="47"/>
+    </row>
+    <row r="85" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C85" s="37"/>
+      <c r="E85" s="53"/>
+      <c r="F85" s="58"/>
+      <c r="G85" s="54"/>
+      <c r="H85" s="53"/>
+      <c r="I85" s="54"/>
+      <c r="J85" s="45"/>
+      <c r="K85" s="47"/>
+      <c r="L85" s="45"/>
+      <c r="M85" s="46"/>
+      <c r="N85" s="47"/>
+    </row>
+    <row r="86" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C86" s="38"/>
+      <c r="E86" s="55"/>
+      <c r="F86" s="59"/>
+      <c r="G86" s="56"/>
+      <c r="H86" s="55"/>
+      <c r="I86" s="56"/>
+      <c r="J86" s="48"/>
+      <c r="K86" s="50"/>
+      <c r="L86" s="48"/>
+      <c r="M86" s="49"/>
+      <c r="N86" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="91">
+    <mergeCell ref="E82:G82"/>
+    <mergeCell ref="H82:I82"/>
+    <mergeCell ref="J82:K82"/>
+    <mergeCell ref="L82:N82"/>
+    <mergeCell ref="E83:G86"/>
+    <mergeCell ref="H83:I86"/>
+    <mergeCell ref="J83:K86"/>
+    <mergeCell ref="L83:N86"/>
+    <mergeCell ref="C74:C86"/>
+    <mergeCell ref="E74:N75"/>
+    <mergeCell ref="E77:F78"/>
+    <mergeCell ref="G77:I78"/>
+    <mergeCell ref="J77:K78"/>
+    <mergeCell ref="L77:N78"/>
+    <mergeCell ref="E79:F80"/>
+    <mergeCell ref="G79:I80"/>
+    <mergeCell ref="J79:K80"/>
+    <mergeCell ref="L79:N80"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="L65:N65"/>
+    <mergeCell ref="E66:G69"/>
+    <mergeCell ref="H66:I69"/>
+    <mergeCell ref="J66:K69"/>
+    <mergeCell ref="L66:N69"/>
+    <mergeCell ref="C57:C69"/>
+    <mergeCell ref="E57:N58"/>
+    <mergeCell ref="E60:F61"/>
+    <mergeCell ref="G60:I61"/>
+    <mergeCell ref="J60:K61"/>
+    <mergeCell ref="L60:N61"/>
+    <mergeCell ref="E62:F63"/>
+    <mergeCell ref="G62:I63"/>
+    <mergeCell ref="J62:K63"/>
+    <mergeCell ref="L62:N63"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="L48:N48"/>
+    <mergeCell ref="E49:G52"/>
+    <mergeCell ref="H49:I52"/>
+    <mergeCell ref="J49:K52"/>
+    <mergeCell ref="L49:N52"/>
+    <mergeCell ref="C40:C52"/>
+    <mergeCell ref="E40:N41"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="G43:I44"/>
+    <mergeCell ref="J43:K44"/>
+    <mergeCell ref="L43:N44"/>
+    <mergeCell ref="E45:F46"/>
+    <mergeCell ref="G45:I46"/>
+    <mergeCell ref="J45:K46"/>
+    <mergeCell ref="L45:N46"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="E32:G35"/>
+    <mergeCell ref="H32:I35"/>
+    <mergeCell ref="J32:K35"/>
+    <mergeCell ref="L32:N35"/>
+    <mergeCell ref="C23:C35"/>
+    <mergeCell ref="E23:N24"/>
+    <mergeCell ref="E26:F27"/>
+    <mergeCell ref="G26:I27"/>
+    <mergeCell ref="J26:K27"/>
+    <mergeCell ref="L26:N27"/>
+    <mergeCell ref="E28:F29"/>
+    <mergeCell ref="G28:I29"/>
+    <mergeCell ref="J28:K29"/>
+    <mergeCell ref="L28:N29"/>
+    <mergeCell ref="L11:N12"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="E15:G18"/>
+    <mergeCell ref="H15:I18"/>
+    <mergeCell ref="J15:K18"/>
+    <mergeCell ref="L15:N18"/>
+    <mergeCell ref="D1:N4"/>
+    <mergeCell ref="C6:C18"/>
+    <mergeCell ref="E6:N7"/>
+    <mergeCell ref="E9:F10"/>
+    <mergeCell ref="G9:I10"/>
+    <mergeCell ref="J9:K10"/>
+    <mergeCell ref="L9:N10"/>
+    <mergeCell ref="E11:F12"/>
+    <mergeCell ref="G11:I12"/>
+    <mergeCell ref="J11:K12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>